<commit_message>
for local run (add test email acc)
</commit_message>
<xml_diff>
--- a/control-tower/src/main/resources/output/file.xlsx
+++ b/control-tower/src/main/resources/output/file.xlsx
@@ -7,17 +7,15 @@
   </bookViews>
   <sheets>
     <sheet name="Lviv Online" r:id="rId3" sheetId="1"/>
-    <sheet name="Gastroli" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'Lviv Online'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Gastroli!$A$1:$F$1</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="287">
   <si>
     <t>Назва</t>
   </si>
@@ -358,6 +356,15 @@
     <t>Перший конгрес — «Перехід 1989» — хронологічно та метафорично відштовхується від 1989 року. Він матиме три тематичні блоки, в рамках яких відбуватимуться дискусії: Мури. Міри. Наміри. Учасники конгресу спробують спільно означити, як і що змінилося у культурній ситуації незалежної України</t>
   </si>
   <si>
+    <t>Вистава «Королева краси»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2018/05/afisha-koroleva-krasy.jpg</t>
+  </si>
+  <si>
+    <t>Тема периферійної, ізольованої людини, яка прагне омріяного життя, але не в змозі його досягнути. Через страхи минулого, що переносяться на реальність, нездатність реалізовувати свої мрії, це бажане життя залишається непрожитим</t>
+  </si>
+  <si>
     <t>Екскурсія «Софіївка + Шевченкове + Вінницький фонтан»</t>
   </si>
   <si>
@@ -457,6 +464,15 @@
     <t>Ви, напевно, бачили ці мальовані плакати на сітілайтах Львова. Видатні львів’яни, які прославили наше місто. Люди різних професій, національностей, поглядів. Вони ходили вулицями Львова в різні часи, але всі залишилися в його пам’яті</t>
   </si>
   <si>
+    <t>Вистава «Апокрифи»</t>
+  </si>
+  <si>
+    <t>2019-10-18T19:00</t>
+  </si>
+  <si>
+    <t>Це низка історій, об'єднаних темою. Підкреслюється одна лінія. Звичайно, при такій побудові детальна розробка нюансів, психологізм образів змінюється виділенням якоїсь однієї риси.</t>
+  </si>
+  <si>
     <t>Екскурсія-тур «Сиро-Винний тур Закарпаттям»</t>
   </si>
   <si>
@@ -472,6 +488,18 @@
     <t>Палац Шенборна, Мукачівський замок, басейн в Берегово, дегустації вина та сиру, водоспат Шипіт та озеро Синевир - все найкраще у Закарпатті. Тривалість туру - 2 дні</t>
   </si>
   <si>
+    <t>Вистава «Забави для Фауста»</t>
+  </si>
+  <si>
+    <t>2019-10-19T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2010/05/afisha_zabavy_dya_fausta.png</t>
+  </si>
+  <si>
+    <t>«Забави для Фауста» — забави вишукані та витончені, де чорно-золотий Свидригайлов бавиться з ляльками</t>
+  </si>
+  <si>
     <t>Виставка Богдана Сороки «Графіка»</t>
   </si>
   <si>
@@ -517,6 +545,18 @@
     <t>Виставка творів яскравої представниці «наївного» мистецтва Марії Примаченко. Понад шістдесят робіт із приватної колекції (Київ) та зі збірки Національного музею у Львові ім. Андрея Шептицького репрезентують її мистецький спадок 1960–1990-х років</t>
   </si>
   <si>
+    <t>Вистава «Маркіза de Sade»</t>
+  </si>
+  <si>
+    <t>2019-10-20T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/05/afisha-vystava-markiza-de-sade.jpg</t>
+  </si>
+  <si>
+    <t>Чи справді жорстокість є невід’ємною частиною природи людини, а темні бажання керують її вчинками? Чи можна прийняти твердження, що гріх та надмірність ведуть до очищення і звільнення?</t>
+  </si>
+  <si>
     <t>Акустичний концерт гурту The Hardkiss</t>
   </si>
   <si>
@@ -529,6 +569,18 @@
     <t>Особлива атмосфера, понад п’ятнадцяти музикантів-мультиінструменталістів на сцені та головні пісні гурту The Hardkiss в новому звучанні. Головні хіти гурту пролунають в несподіваних аранжуваннях в акустиці завдяки класичним та народним інструментам</t>
   </si>
   <si>
+    <t>Вистава «Ножі в курях, або Спадок мірошника»</t>
+  </si>
+  <si>
+    <t>2019-10-23T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2016/02/afisha-vystava-nozhi-v-kuriakh.jpg</t>
+  </si>
+  <si>
+    <t>Вистава за п'єсою сучасного шотландського драматурга Девіда Гарровера «Ножі в курях»</t>
+  </si>
+  <si>
     <t>Екскурсія-тур «10 родзинок Закарпаття»</t>
   </si>
   <si>
@@ -544,6 +596,18 @@
     <t>Карпати, замки, палаци, вина, все найкраще, що може запропонувати гостинне Закарпаття, чекає на Вас. Тривалість туру - 3 дні</t>
   </si>
   <si>
+    <t>Вистава «Лісова пісня»</t>
+  </si>
+  <si>
+    <t>2019-10-25T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2011/02/afisha_lisova_pisnya_kurbasa.jpg</t>
+  </si>
+  <si>
+    <t>Вистава за п'єсою Лесі Українки у трьох колядах (за підтримки Благодійного Фонду «Розвиток України»). У виставі використані пісні фольклорних гуртів «Кросна», «Божичі», «Древо».</t>
+  </si>
+  <si>
     <t>Екскурсія-тур «Сплав по Черемошу і не лише»</t>
   </si>
   <si>
@@ -571,6 +635,18 @@
     <t>Запрошуємо піднятися на найвищу вершину в Україні, а також побачити фантастичні гірські пейзажі та водоспади. Тривалість туру - 2 дні</t>
   </si>
   <si>
+    <t>Вистава «Формули екстази»</t>
+  </si>
+  <si>
+    <t>2019-10-26T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2009/10/antonych_formuly.jpg</t>
+  </si>
+  <si>
+    <t>Вистава «Формули екстази» є драматичними замальовками за текстами Богдана Ігоря Антонича та Луїджі Піранделло. Режисером вистави є Олег Цьона.</t>
+  </si>
+  <si>
     <t>Концерт гурту The Rasmus</t>
   </si>
   <si>
@@ -586,6 +662,18 @@
     <t>Чорний одяг, мейк-ап, пісня «In the Shadows» в навушниках. Відчули приємну ностальгію? Найвідоміша група Фінляндії: дев’ять студійних альбомів, величезна кількість музичних нагород, любов армії шанувальників і культовий статус в історії рок-музики нульових</t>
   </si>
   <si>
+    <t>Вистава «Так казав Заратустра»</t>
+  </si>
+  <si>
+    <t>2019-10-27T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2012/12/afisha_tak_kazav_zaratustra.jpg</t>
+  </si>
+  <si>
+    <t>Проект орієнтовано насамперед на пошук духовних джерел, драйву життя через форми слова, пластики, співу, візуального оформлення. Спроба перенести думки Ніцше/Заратустри у сьогоднішні українські реалії</t>
+  </si>
+  <si>
     <t>Музично-танцювальне шоу Ladies Night</t>
   </si>
   <si>
@@ -712,99 +800,6 @@
     <t>В процесі створення альбому з групи пішли гітарист і басист. Альбом «Таємний код» скдається з двох частин, в якому вперше за 15 років існування гурту «Бумбокс» буде більше 11 пісень. Три з них добре тобі знайомі і стали суперхітами</t>
   </si>
   <si>
-    <t>Концерт гурту Karna</t>
-  </si>
-  <si>
-    <t>!FESTrepublic</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2018/07/afisha-karna-gucul.jpg</t>
-  </si>
-  <si>
-    <t>Гурт із 20-річною історією за цей значний відтинок часу пережив три транформації і навіть цілковитий розпад. Прихід до гурту нового соліста Олексія Шманьова був ознаменований створенням модернового музичного стилю – «гуцул-метал»</t>
-  </si>
-  <si>
-    <t>Клубний концерт HammAli &amp; Navai</t>
-  </si>
-  <si>
-    <t>2019-11-28T20:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-HammAli-Navai.jpg</t>
-  </si>
-  <si>
-    <t>Танцювальні треки з елементами хаусу, діпу й пронизливою, душевною реп-лірикою стрімко завойовують любов фанів. Минулого року HammAli &amp; Navai викликали справжній хайп. Цьогоріч музичні інфлюенсери пообіцяли зробити тусу для своїх ще крутішою</t>
-  </si>
-  <si>
-    <t>Концерт Metallica Symphonic Tribute</t>
-  </si>
-  <si>
-    <t>2019-12-02T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-Metallica-Symphonic-Tribute.jpeg</t>
-  </si>
-  <si>
-    <t>З 2015 року почалася підготовка симфонічного Metallica Tribute Show під керівництвом досвідчених концертних промоутерів. Гурт почав гастролювати з симфонічним оркестром, продовжуючи розвивати оригінальну програму. Однак проект досяг своєї пікової позиції тільки зараз</t>
-  </si>
-  <si>
-    <t>Вистава « №13 або ОлІнклюзив»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2015/09/afisha-allinclusive.jpg</t>
-  </si>
-  <si>
-    <t>Ексцентрична театральна комедія Рея Куні. Здавалося б знайомий сюжет: секретарка опозиційної партії і впливовий політик в одному номері. І як тільки побачення підходить до кульмінації…</t>
-  </si>
-  <si>
-    <t>Виступ гурту Heilung</t>
-  </si>
-  <si>
-    <t>2019-12-06T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/04/afisha-Heilung.jpg</t>
-  </si>
-  <si>
-    <t>Heilung - автори саундтреків до останнього сезону «Гри престолів». Вперше данська неофолк група Heilung привезе в Україну театралізоване музичне шоу у ритмі шаманів та бойових пісень вікінгів</t>
-  </si>
-  <si>
-    <t>Гурт Ost+Front (DE) презентує альбом Adrenalin</t>
-  </si>
-  <si>
-    <t>2019-12-07T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-ost-front.jpg</t>
-  </si>
-  <si>
-    <t>Легенди напрямку Neue Deutsche Härte німецький гурт Ost+Front вперше завітають до Львова з презентацією альбому Adrenalin та кращими хітами за всі роки. Гурт був заснований в 2008 році в Берліні колишнім учасником групи Tanzwut Патріком Ланг</t>
-  </si>
-  <si>
-    <t>Скрябін. Концерт до 30-річного ювілею гурту</t>
-  </si>
-  <si>
-    <t>2019-12-23T20:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-skriabin-urkesh.jpg</t>
-  </si>
-  <si>
-    <t>Улюблені пісні у виконанні гурту «Скрябін» і лідера гурту «Юркеш» Юрка Юрченка. Незвичне звучання хітів Кузьми у супроводі симфонічного оркестру. Спеціальний відео і фоторяд на великому екрані, історії з життя і про життя Кузьми</t>
-  </si>
-  <si>
-    <t>Концерт Lords Of The Sound з програмою Grand Christmas</t>
-  </si>
-  <si>
-    <t>2019-12-25T19:30</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-Lords-of-the-Sound-grand-christmas.jpg</t>
-  </si>
-  <si>
-    <t>Grand Christmas – це не просто концерт, а справжня різдвяна казка у котру зможуть потрапити гості свята. Lords of the Sound готують неймовірну музичну програму із європейських різдвяних хітів та саундтреків до ваших улюблених новорічних фільмів</t>
-  </si>
-  <si>
     <t>2019-09-30 19:00</t>
   </si>
   <si>
@@ -838,12 +833,33 @@
     <t>2019-10-14 19:00</t>
   </si>
   <si>
+    <t>2019-10-18 19:00</t>
+  </si>
+  <si>
+    <t>2019-10-19 19:00</t>
+  </si>
+  <si>
+    <t>2019-10-20 19:00</t>
+  </si>
+  <si>
     <t>2019-10-21 19:00</t>
   </si>
   <si>
+    <t>2019-10-23 19:00</t>
+  </si>
+  <si>
+    <t>2019-10-25 19:00</t>
+  </si>
+  <si>
+    <t>2019-10-26 19:00</t>
+  </si>
+  <si>
     <t>2019-10-27 20:00</t>
   </si>
   <si>
+    <t>2019-10-27 19:00</t>
+  </si>
+  <si>
     <t>2019-10-29 20:00</t>
   </si>
   <si>
@@ -860,24 +876,6 @@
   </si>
   <si>
     <t>2019-11-22 19:00</t>
-  </si>
-  <si>
-    <t>2019-11-28 20:00</t>
-  </si>
-  <si>
-    <t>2019-12-02 19:00</t>
-  </si>
-  <si>
-    <t>2019-12-06 19:00</t>
-  </si>
-  <si>
-    <t>2019-12-07 19:00</t>
-  </si>
-  <si>
-    <t>2019-12-23 20:00</t>
-  </si>
-  <si>
-    <t>2019-12-25 19:30</t>
   </si>
 </sst>
 </file>
@@ -885,18 +883,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -962,7 +955,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="363">
+  <cellXfs count="371">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
       <alignment horizontal="left"/>
@@ -2008,24 +2001,60 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFont="true" applyFill="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -2045,7 +2074,7 @@
     <col min="2" max="2" width="22.9453125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="19.6953125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="108.6484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="94.7734375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="92.57421875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2094,7 +2123,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s" s="18">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s" s="19">
         <v>14</v>
@@ -2234,7 +2263,7 @@
         <v>44</v>
       </c>
       <c r="B10" t="s" s="60">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C10" t="s" s="61">
         <v>14</v>
@@ -2294,7 +2323,7 @@
         <v>58</v>
       </c>
       <c r="B13" t="s" s="78">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C13" t="s" s="79">
         <v>20</v>
@@ -2314,7 +2343,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s" s="84">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C14" t="s" s="85">
         <v>20</v>
@@ -2334,7 +2363,7 @@
         <v>67</v>
       </c>
       <c r="B15" t="s" s="90">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s" s="91">
         <v>14</v>
@@ -2374,7 +2403,7 @@
         <v>75</v>
       </c>
       <c r="B17" t="s" s="102">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C17" t="s" s="103">
         <v>14</v>
@@ -2394,7 +2423,7 @@
         <v>79</v>
       </c>
       <c r="B18" t="s" s="108">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C18" t="s" s="109">
         <v>14</v>
@@ -2454,7 +2483,7 @@
         <v>93</v>
       </c>
       <c r="B21" t="s" s="126">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C21" t="s" s="127">
         <v>95</v>
@@ -2471,430 +2500,430 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="131">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s" s="132">
-        <v>270</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s" s="133">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s" s="134">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s" s="135">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F22" t="s" s="136">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="137">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s" s="138">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s" s="139">
         <v>8</v>
       </c>
       <c r="D23" t="s" s="140">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s" s="141">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s" s="142">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="143">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s" s="144">
-        <v>110</v>
+        <v>268</v>
       </c>
       <c r="C24" t="s" s="145">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s" s="146">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s" s="147">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F24" t="s" s="148">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="149">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s" s="150">
-        <v>110</v>
+        <v>269</v>
       </c>
       <c r="C25" t="s" s="151">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s" s="152">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s" s="153">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="F25" t="s" s="154">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="155">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s" s="156">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s" s="157">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s" s="158">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s" s="159">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="F26" t="s" s="160">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="161">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s" s="162">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s" s="163">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s" s="164">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s" s="165">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s" s="166">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="167">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s" s="168">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C28" t="s" s="169">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s" s="170">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s" s="171">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="F28" t="s" s="172">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="173">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s" s="174">
-        <v>272</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s" s="175">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s" s="176">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="E29" t="s" s="177">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="F29" t="s" s="178">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="179">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s" s="180">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s" s="181">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D30" t="s" s="182">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E30" t="s" s="183">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="F30" t="s" s="184">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="185">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s" s="186">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s" s="187">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s" s="188">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E31" t="s" s="189">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="F31" t="s" s="190">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="191">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B32" t="s" s="192">
-        <v>147</v>
+        <v>270</v>
       </c>
       <c r="C32" t="s" s="193">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s" s="194">
-        <v>148</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s" s="195">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="F32" t="s" s="196">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="197">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s" s="198">
-        <v>152</v>
+        <v>271</v>
       </c>
       <c r="C33" t="s" s="199">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s" s="200">
-        <v>153</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s" s="201">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="F33" t="s" s="202">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="203">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s" s="204">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C34" t="s" s="205">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s" s="206">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E34" t="s" s="207">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="F34" t="s" s="208">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="209">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B35" t="s" s="210">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C35" t="s" s="211">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s" s="212">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E35" t="s" s="213">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="F35" t="s" s="214">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="215">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s" s="216">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C36" t="s" s="217">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s" s="218">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E36" t="s" s="219">
-        <v>168</v>
+        <v>34</v>
       </c>
       <c r="F36" t="s" s="220">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="221">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s" s="222">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C37" t="s" s="223">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s" s="224">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="E37" t="s" s="225">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="F37" t="s" s="226">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="227">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B38" t="s" s="228">
-        <v>176</v>
+        <v>273</v>
       </c>
       <c r="C38" t="s" s="229">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s" s="230">
-        <v>177</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s" s="231">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="F38" t="s" s="232">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="233">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="B39" t="s" s="234">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s" s="235">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s" s="236">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="E39" t="s" s="237">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="F39" t="s" s="238">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="239">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s" s="240">
-        <v>274</v>
+        <v>167</v>
       </c>
       <c r="C40" t="s" s="241">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s" s="242">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E40" t="s" s="243">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="F40" t="s" s="244">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="245">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B41" t="s" s="246">
-        <v>275</v>
+        <v>172</v>
       </c>
       <c r="C41" t="s" s="247">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s" s="248">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="E41" t="s" s="249">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="F41" t="s" s="250">
-        <v>192</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="251">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="B42" t="s" s="252">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="C42" t="s" s="253">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D42" t="s" s="254">
-        <v>194</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s" s="255">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="F42" t="s" s="256">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="257">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="B43" t="s" s="258">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C43" t="s" s="259">
         <v>14</v>
@@ -2903,355 +2932,370 @@
         <v>15</v>
       </c>
       <c r="E43" t="s" s="261">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="F43" t="s" s="262">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="263">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="B44" t="s" s="264">
-        <v>202</v>
+        <v>276</v>
       </c>
       <c r="C44" t="s" s="265">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D44" t="s" s="266">
-        <v>203</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s" s="267">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="F44" t="s" s="268">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="269">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B45" t="s" s="270">
-        <v>277</v>
+        <v>189</v>
       </c>
       <c r="C45" t="s" s="271">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s" s="272">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="E45" t="s" s="273">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="F45" t="s" s="274">
-        <v>209</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="275">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="B46" t="s" s="276">
-        <v>211</v>
+        <v>277</v>
       </c>
       <c r="C46" t="s" s="277">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="D46" t="s" s="278">
-        <v>212</v>
+        <v>33</v>
       </c>
       <c r="E46" t="s" s="279">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="F46" t="s" s="280">
-        <v>214</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="281">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s" s="282">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C47" t="s" s="283">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D47" t="s" s="284">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="E47" t="s" s="285">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F47" t="s" s="286">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="287">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="B48" t="s" s="288">
-        <v>278</v>
+        <v>198</v>
       </c>
       <c r="C48" t="s" s="289">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s" s="290">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="E48" t="s" s="291">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="F48" t="s" s="292">
-        <v>222</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="293">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B49" t="s" s="294">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C49" t="s" s="295">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D49" t="s" s="296">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s" s="297">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="F49" t="s" s="298">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="299">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="B50" t="s" s="300">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C50" t="s" s="301">
         <v>14</v>
       </c>
       <c r="D50" t="s" s="302">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="E50" t="s" s="303">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="F50" t="s" s="304">
-        <v>230</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="305">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B51" t="s" s="306">
         <v>280</v>
       </c>
       <c r="C51" t="s" s="307">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D51" t="s" s="308">
-        <v>232</v>
+        <v>33</v>
       </c>
       <c r="E51" t="s" s="309">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="F51" t="s" s="310">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="311">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B52" t="s" s="312">
         <v>281</v>
       </c>
       <c r="C52" t="s" s="313">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D52" t="s" s="314">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="E52" t="s" s="315">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="F52" t="s" s="316">
-        <v>238</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="317">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="B53" t="s" s="318">
-        <v>282</v>
+        <v>167</v>
       </c>
       <c r="C53" t="s" s="319">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s" s="320">
-        <v>15</v>
+        <v>224</v>
       </c>
       <c r="E53" t="s" s="321">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="F53" t="s" s="322">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="323">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B54" t="s" s="324">
         <v>282</v>
       </c>
       <c r="C54" t="s" s="325">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D54" t="s" s="326">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E54" t="s" s="327">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="F54" t="s" s="328">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="329">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B55" t="s" s="330">
-        <v>283</v>
+        <v>232</v>
       </c>
       <c r="C55" t="s" s="331">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s" s="332">
-        <v>60</v>
+        <v>233</v>
       </c>
       <c r="E55" t="s" s="333">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="F55" t="s" s="334">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="335">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B56" t="s" s="336">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C56" t="s" s="337">
         <v>14</v>
       </c>
       <c r="D56" t="s" s="338">
-        <v>232</v>
+        <v>29</v>
       </c>
       <c r="E56" t="s" s="339">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="F56" t="s" s="340">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="341">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B57" t="s" s="342">
-        <v>285</v>
+        <v>241</v>
       </c>
       <c r="C57" t="s" s="343">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="D57" t="s" s="344">
-        <v>15</v>
+        <v>242</v>
       </c>
       <c r="E57" t="s" s="345">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="F57" t="s" s="346">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="347">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B58" t="s" s="348">
+        <v>241</v>
+      </c>
+      <c r="C58" t="s" s="349">
+        <v>117</v>
+      </c>
+      <c r="D58" t="s" s="350">
+        <v>246</v>
+      </c>
+      <c r="E58" t="s" s="351">
+        <v>247</v>
+      </c>
+      <c r="F58" t="s" s="352">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="353">
+        <v>249</v>
+      </c>
+      <c r="B59" t="s" s="354">
+        <v>284</v>
+      </c>
+      <c r="C59" t="s" s="355">
+        <v>14</v>
+      </c>
+      <c r="D59" t="s" s="356">
+        <v>101</v>
+      </c>
+      <c r="E59" t="s" s="357">
+        <v>251</v>
+      </c>
+      <c r="F59" t="s" s="358">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="359">
+        <v>253</v>
+      </c>
+      <c r="B60" t="s" s="360">
+        <v>285</v>
+      </c>
+      <c r="C60" t="s" s="361">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s" s="362">
+        <v>29</v>
+      </c>
+      <c r="E60" t="s" s="363">
+        <v>255</v>
+      </c>
+      <c r="F60" t="s" s="364">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="365">
+        <v>257</v>
+      </c>
+      <c r="B61" t="s" s="366">
         <v>286</v>
       </c>
-      <c r="C58" t="s" s="349">
+      <c r="C61" t="s" s="367">
         <v>14</v>
       </c>
-      <c r="D58" t="s" s="350">
-        <v>29</v>
-      </c>
-      <c r="E58" t="s" s="351">
+      <c r="D61" t="s" s="368">
+        <v>101</v>
+      </c>
+      <c r="E61" t="s" s="369">
+        <v>259</v>
+      </c>
+      <c r="F61" t="s" s="370">
         <v>260</v>
-      </c>
-      <c r="F58" t="s" s="352">
-        <v>261</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F1"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <tabColor indexed="17"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="6.49609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.5859375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.31640625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="18.4609375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="22.94140625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.7578125" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="40.0" customHeight="true">
-      <c r="A1" t="s" s="355">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="355">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="355">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="355">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="355">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="355">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
for local run (gastroli)
</commit_message>
<xml_diff>
--- a/control-tower/src/main/resources/output/file.xlsx
+++ b/control-tower/src/main/resources/output/file.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="208">
   <si>
     <t>Назва</t>
   </si>
@@ -35,544 +35,448 @@
     <t>Опис</t>
   </si>
   <si>
-    <t>Виставка Дарії Зав’ялової «Забуті вілли»</t>
-  </si>
-  <si>
-    <t>2019-09-01</t>
+    <t>Виступ гурту Heilung</t>
+  </si>
+  <si>
+    <t>2019-12-06T19:00</t>
+  </si>
+  <si>
+    <t>МУЗИКА</t>
+  </si>
+  <si>
+    <t>Львівський державний цирк</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/04/afisha-Heilung.jpg</t>
+  </si>
+  <si>
+    <t>Heilung - автори саундтреків до останнього сезону «Гри престолів». Вперше данська неофолк група Heilung привезе в Україну театралізоване музичне шоу у ритмі шаманів та бойових пісень вікінгів</t>
+  </si>
+  <si>
+    <t>Вистава «В гості до Сонечка». ПРЕМ’ЄРА!</t>
+  </si>
+  <si>
+    <t>2019-12-06T12:00</t>
+  </si>
+  <si>
+    <t>ТЕАТР</t>
+  </si>
+  <si>
+    <t>Львівський академічний театр естрадних мініатюр «І люди, і ляльки»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/10/vystava-v-hosti-do-sonechka.jpg</t>
+  </si>
+  <si>
+    <t>Одного разу Сонечко не з'явилось на небі і двоє маленьких курчат вирішили з'ясувати причину такої поведінки і вирушили до Сонечка в гості</t>
+  </si>
+  <si>
+    <t>Вистава «Dogs»</t>
+  </si>
+  <si>
+    <t>2019-12-06T13:00</t>
+  </si>
+  <si>
+    <t>Перший театр</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2016/03/afisha-vystava-dog.jpg</t>
+  </si>
+  <si>
+    <t>Проста і чуйна історія про собак і людей, історія, яка закликає до людяності і добра. Вистава спонукає замислиться над життям безпритульних тварин. Адже усі ми шукаємо Свою Людину і свої дверцята до щастя</t>
+  </si>
+  <si>
+    <t>Гурт Ost+Front (DE) презентує альбом Adrenalin</t>
+  </si>
+  <si>
+    <t>2019-12-07T19:00</t>
+  </si>
+  <si>
+    <t>!FESTrepublic</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-ost-front.jpg</t>
+  </si>
+  <si>
+    <t>Легенди напрямку Neue Deutsche Härte німецький гурт Ost+Front вперше завітають до Львова з презентацією альбому Adrenalin та кращими хітами за всі роки. Гурт був заснований в 2008 році в Берліні колишнім учасником групи Tanzwut Патріком Ланг</t>
+  </si>
+  <si>
+    <t>Вистава «Небезпечна гра»</t>
+  </si>
+  <si>
+    <t>2019-12-07T17:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2015/03/afisha_nebezpechna_hra.jpg</t>
+  </si>
+  <si>
+    <t>Жіноча сповідь і маніфест свободи, це історія про двох жінок – авантюрної пенсіонерки та революційно налаштованої проти минулого, котрі вирішують йди ва-банк і розпочинають свою гру із життям</t>
+  </si>
+  <si>
+    <t>Вистава «…п’єса Шекспіра «12 ніч», зіграна акторами далекої від Англії країни, що і не знали ніколи слів Шекспіра…»</t>
+  </si>
+  <si>
+    <t>Львівський академічний театр ім. Леся Курбаса</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2014/11/afisha_12_nich.jpg</t>
+  </si>
+  <si>
+    <t>Це буде одна дуже стара історія. Ті хто їх розказують - змінюють імена, героїв країни, де вони відбувалися. Іноді їм здається що це вони, вони перші розказали про кохання щось таке, чого світ до них не знав</t>
+  </si>
+  <si>
+    <t>Вистава «Одного разу в Африці…»</t>
+  </si>
+  <si>
+    <t>2019-12-07T12:00, 14:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2013/04/afisha_odnoho_razu_afryci.jpg</t>
+  </si>
+  <si>
+    <t>Головні герої вистави — Жирафа і Носоріг, які попри різницю у своїй вроді, зуміли подружитися. Історія їхньої дружби — це приклад того, наскільки важливими є внутрішні переваги будь-якого живого створіння</t>
+  </si>
+  <si>
+    <t>Опера «Ріголетто»</t>
+  </si>
+  <si>
+    <t>2019-12-07T18:00</t>
+  </si>
+  <si>
+    <t>Львівський національний академічний театр опери та балету ім. Соломії Крушельницької</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2009/12/opera-riholetto.jpg</t>
+  </si>
+  <si>
+    <t>Подвійне життя веде Ріголетто. При дворі він - охочий виконавець волі пана, в маленькому будиночку далеко від палацу — ніжний батько, що береже від усього світу свою доньку Джільду.</t>
+  </si>
+  <si>
+    <t>Вистава «Пауза»</t>
+  </si>
+  <si>
+    <t>2019-12-08T18:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/11/afisha-vystavva-pauza.jpg</t>
+  </si>
+  <si>
+    <t>Через призму особистих історій, думок та рефлексій учасників-акторів вистава говоритиме про наше з вами повсякденне життя. Пора зробити ПАУЗУ і поглянути туди, униз, убік, уверх - через завісу притертої повсякденності. Як ми виглядатимемо без своєї звичної шкіри?</t>
+  </si>
+  <si>
+    <t>Виставка Дарії Зав’ялової «Місто і сад»</t>
+  </si>
+  <si>
+    <t>2019-11-19</t>
   </si>
   <si>
     <t>МИСТЕЦТВО</t>
   </si>
   <si>
-    <t>Кав’ярня «Штука»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-dariya-zavialova.jpg</t>
-  </si>
-  <si>
-    <t>Виставка пастелей Дарії Зав’ялової «Забуті вілли». 30 років творчого життя працювала художником театру. Поза театром працює в сфері художнього текстилю, останні 10 років малює Львів (акрил, акварель, пастель)</t>
-  </si>
-  <si>
-    <t>Концерт піаніста Peter Bence</t>
-  </si>
-  <si>
-    <t>2019-09-30T19:00</t>
-  </si>
-  <si>
-    <t>МУЗИКА</t>
-  </si>
-  <si>
-    <t>Львівський національний академічний театр опери та балету ім. Соломії Крушельницької</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-Peter-Bence.jpg</t>
-  </si>
-  <si>
-    <t>Піаніст внесений до Книги рекордів Гіннеса, як піаніст-рекордсмен з швидкості повторюваного натизку (репетиції) однієї клавіші (765 клавіш на хвилину). Його версію хітів Майкла Джексона побачило більше 40 мільйонів глядачів</t>
-  </si>
-  <si>
-    <t>Виставка Hortus Conclusus</t>
-  </si>
-  <si>
-    <t>2019-06-25</t>
-  </si>
-  <si>
-    <t>ІНШЕ</t>
-  </si>
-  <si>
-    <t>Львівський музей історії релігії</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/06/afisha-Hortus-Conclusus.jpg</t>
-  </si>
-  <si>
-    <t>Понад три десятки рослин представлено у внутрішньому дворику музею на виставці Hortus Conclusus. Серед добре відомих і впізнаваних рослин у саду ростуть ялівець, плющ, півники, шипшина, фінікова пальма, лілея, м’ята, самшит (букшпан)</t>
-  </si>
-  <si>
-    <t>Театр опери та балету ім. Соломії Крушельницької. Репертуар на вересень 2019</t>
-  </si>
-  <si>
-    <t>ТЕАТР</t>
+    <t>Мистецька галерея «Зелена Канапа»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/11/afisha-misto-i-sad.jpg</t>
+  </si>
+  <si>
+    <t>Місто і Сад не суперечать одне одному. Вони доповнюють гармонію рукотворну і природню. Місто своєю архітектурою – прекрасним зодчеством кам’яних окультурених «печер», місць куди можна сховатись для відчуття безпеки і захисту від негоди</t>
+  </si>
+  <si>
+    <t>Виставка Романа Романишина «Перехрестя»</t>
+  </si>
+  <si>
+    <t>2019-11-08</t>
+  </si>
+  <si>
+    <t>Національний музей у Львові ім. Андрея Шептицького</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/11/afisha-romanyshyn-perehrestia.jpg</t>
+  </si>
+  <si>
+    <t>Секрет успіху Романа Романишина як художника криється в дивному поєднанні власного внутрішнього світу, безконечного поля спогадів, сформованого на рівні дитячих уявлень, з глибоко індивідуальними переживаннями актуальних подій сьогодення</t>
+  </si>
+  <si>
+    <t>Вистава «Танець життя»</t>
+  </si>
+  <si>
+    <t>Львівський академічний духовний театр «Воскресіння»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2016/02/afisha-vystava-tanets-zhyttia.jpg</t>
+  </si>
+  <si>
+    <t>Вистава класика української драматургії Олександра Олеся, яка включає чотири одноактні п’єси: «Танець життя», «По Мюллеру», «Юність» та «Патріот». Вистава різножанрова, де переплітаються комедія, драма, трагедія, водевіль</t>
+  </si>
+  <si>
+    <t>Вистава «Хто сказав «Няв»</t>
+  </si>
+  <si>
+    <t>2019-12-08T12:00, 14:00, 16:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2012/11/afisha_hto_skazav_njav.jpg</t>
+  </si>
+  <si>
+    <t>Для самих маленьких глядачів яскрава вистава-мініатюра, яка вводить малят у світ живих тваринок, вчить з ними розмовляти, контактувати, дає дитині психологічні уроки дружби і рівноваги</t>
+  </si>
+  <si>
+    <t>Балет «Лускунчик»</t>
+  </si>
+  <si>
+    <t>2019-12-08T12:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2009/11/balet-luskunchyk.jpg</t>
+  </si>
+  <si>
+    <t>Різдвяний вечір. Майстер ляльок Дроссельмейєр показує дівчині своє царство ляльок. Всі вони надзвичайні й наче живі. Маші найбільше сподобалася кумедна іграшка, шо вміє лускати горіхи.</t>
+  </si>
+  <si>
+    <t>Вистава «Лялька Реґґеді Енн»</t>
+  </si>
+  <si>
+    <t>2019-12-10T12:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2012/01/afisha-lialka-regeddi-enn.jpeg</t>
+  </si>
+  <si>
+    <t>Маловідомий для нас, але знаковий для дитячої американької культури персонаж Реґґеді Енн (Raggedy Ann) – простенька лялька, вигадана і намальована письменником Джоном Ґруелом</t>
+  </si>
+  <si>
+    <t>Вистава «Маркіза de Sade»</t>
+  </si>
+  <si>
+    <t>2019-12-11T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/05/afisha-vystava-markiza-de-sade.jpg</t>
+  </si>
+  <si>
+    <t>Чи справді жорстокість є невід’ємною частиною природи людини, а темні бажання керують її вчинками? Чи можна прийняти твердження, що гріх та надмірність ведуть до очищення і звільнення?</t>
+  </si>
+  <si>
+    <t>Вистава «Чоловік моєї дружини»</t>
+  </si>
+  <si>
+    <t>2019-12-11T18:00</t>
+  </si>
+  <si>
+    <t>Театр ім. Марії Заньковецької, камерна сцена</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2017/03/afisha-vystava-cholovik-moiei-druzhyny.jpg</t>
+  </si>
+  <si>
+    <t>Жаркець хороший батько, любить прибирати дім та створювати затишок, Креше – чудовий кухар й пристрасний коханець. Ідеал чоловіка, поділений на двоє і, можливо, єдиний варіант для розумної жінки аби жити у гармонії</t>
+  </si>
+  <si>
+    <t>Вистава «Проданий сміх»</t>
+  </si>
+  <si>
+    <t>2019-12-12T13:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2018/12/afisha-prodanyi-smih.jpg</t>
+  </si>
+  <si>
+    <t>Філософську повість-казку «Тім Талер або проданий сміх» часто називають Фаустом для дітей. Це історія про веселу дитину, що проміняла свій сміх на здатність вигравати будь-який заклад</t>
+  </si>
+  <si>
+    <t>Вистава «Катерина»</t>
+  </si>
+  <si>
+    <t>2019-12-12T18:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2012/12/afisha_kateryna.jpg</t>
+  </si>
+  <si>
+    <t>Світ Шевченкової «Катерина» очима режисера Богдана Ревкевича. До уваги глядачів особлива історія, особливої жінки, яка шукала дивних скарбів, а знайшла тяжку ношу</t>
+  </si>
+  <si>
+    <t>Вистава «Серпень. Графство Осейдж». ПРЕМ’ЄРА!</t>
+  </si>
+  <si>
+    <t>2019-12-13T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/10/afisha-serpen-hrafstvo-oseidzh.jpg</t>
+  </si>
+  <si>
+    <t>Зіткнення поколінь: батьки і діти, нездійсненні мрії, скелети у шафах великого будинку і яскраві характери головних героїв. Ось і вся формула щастя. Саме гра в «любов» приведе персонажів п’єси до ревнощів і заздрості, а згодом і до сімейного краху. Сімейні вузи … що це? Обов’язок чи любов?</t>
+  </si>
+  <si>
+    <t>Вистава «Аліса»</t>
+  </si>
+  <si>
+    <t>2019-12-13T12:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/01/afisha-alisa.jpg</t>
+  </si>
+  <si>
+    <t>Фантасмагорична подорож у глибини власного Я: чим дивніше, тим видніше! Постановка з елементами тіньового театру. Завдяки комбінованому сценічному простору герої вистави вільно переміщаються у світ тіней та назад</t>
+  </si>
+  <si>
+    <t>Вистава «Горизонт 200»</t>
+  </si>
+  <si>
+    <t>2019-12-13T18:00</t>
+  </si>
+  <si>
+    <t>Львівський академічний драматичний театр ім. Лесі Українки</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2018/12/afisha-vystava-horyzont-200.jpg</t>
+  </si>
+  <si>
+    <t>Вистава не про шахту, а про кожного з нас. «Горизонт 200» - так шахтарі кажуть про глибину дві тисячі метрів під землею; для нас це і про дві тисячі кілометрів України з півночі на південь, зі сходу на захід; це про нашу можливість бачити і небажання дивитися</t>
+  </si>
+  <si>
+    <t>Вистава «Смак до черешень»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2014/04/afisha-smak-do-chereshen.jpg</t>
+  </si>
+  <si>
+    <t>Вистава «Смак до черешень» А. Осецької. Режисер-постановник - Галина Воловецька, художник-постановник - Наталя Тарасенко</t>
+  </si>
+  <si>
+    <t>Вистава «Шовкова косиця»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2012/12/shovkova_kosycya.jpg</t>
+  </si>
+  <si>
+    <t>«Шовкова косиця» є свідченням сили артистичного духу, віри і відданості, покликом до кожного із нас, з бажанням бути почутим. Актори, улюбленці малят, працюють і творять світ, невідомий для сильних світу цього.</t>
+  </si>
+  <si>
+    <t>Вистава «Амнезія, або Маленькі подружні злочини»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2010/08/afisha_amneziya_zlochyny_kurbasa.jpg</t>
+  </si>
+  <si>
+    <t>Тренінг акторської імпровізації. Подружні стосунки мусять мати в собі елемент театральності, інакше їм надто швидко загрожує «виснаження почуттів»</t>
+  </si>
+  <si>
+    <t>Вистава «Принцеса і сто поцілунків»</t>
+  </si>
+  <si>
+    <t>2019-12-14T13:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/03/afisha-pryncessa-i-sto-pocilunkiv.jpg</t>
+  </si>
+  <si>
+    <t>Казка для батьків з дітьми. У темному-темному королівстві, де все заборонено, де не можна співати веселих пісень, слухати щебетання птахів та милуватися квітами, живе юна Принцеса</t>
+  </si>
+  <si>
+    <t>Вистава «Мій Роден»</t>
+  </si>
+  <si>
+    <t>2019-12-14T18:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2018/02/afisha-vystava-mij-roden.jpg</t>
+  </si>
+  <si>
+    <t>Відтоді, як Камілла пішла від нього, його скульптури уже не сяяли ніжними почуттями. Його геній, колись розквітлий від цієї зустрічі, тепер дихав рівно, спокійно, без присмаку шаленої творчої пристрасті</t>
+  </si>
+  <si>
+    <t>Вистава «Раптом минулого літа»</t>
+  </si>
+  <si>
+    <t>2019-12-14T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2016/04/afisha-raptom-mynulogo-lita.jpg</t>
+  </si>
+  <si>
+    <t>Тендітна дівчина, яку одні хочуть використати, а інші просто ліквідувати, цілковито позбавлена свободи і прав та має лише один спосіб зберегти те, що їй залишили від життя – збрехати</t>
+  </si>
+  <si>
+    <t>Вистава «Снігова королева»</t>
+  </si>
+  <si>
+    <t>2019-12-14T12:00, 14:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2015/01/afisha_snigova_koroleva.jpg</t>
+  </si>
+  <si>
+    <t>Добре відома нам усім з дитинства казка Ганса Хрістіана Андерсена «Снігова королева». Ця історія розповідає нам про те, як важливо вміти зберегти в своїх серцях щирий, дитячий вогник любові</t>
+  </si>
+  <si>
+    <t>Опера «Лис Микита». ПРЕМ’ЄРА!</t>
+  </si>
+  <si>
+    <t>2019-12-15T12:00, 18:00</t>
   </si>
   <si>
     <t>https://lviv-online.com/ua/wp-content/uploads/2012/11/lviv-opera-logo.jpg</t>
   </si>
   <si>
-    <t>Репертуар вистав Львівського Національного академічного театру опери та балету ім. Соломії Крушельницької на вересень 2019 року</t>
-  </si>
-  <si>
-    <t>Театр ім. Марії Заньковецької. Репертуар на вересень 2019</t>
-  </si>
-  <si>
-    <t>Національний академічний український драматичний театр ім. Марії Заньковецької</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2012/11/teatr-im-marii-zankovetskoi-logo.jpg</t>
-  </si>
-  <si>
-    <t>Репертуар вистав у Національному академічному українському драматичному театрі ім. Марії Заньковецької на вересень 2019 року</t>
-  </si>
-  <si>
-    <t>Театр ім. Леся Курбаса. Репертуар на вересень 2019</t>
-  </si>
-  <si>
-    <t>Львівський академічний театр ім. Леся Курбаса</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2012/10/logo_teatr_kurbasa_lviv.jpg</t>
-  </si>
-  <si>
-    <t>Репертуар вистав Львівського академічного театру ім. Леся Курбаса на вересень 2019 року</t>
-  </si>
-  <si>
-    <t>Львівський театр естрадних мініатюр «І люди, і ляльки». Репертуар на вересень 2019</t>
-  </si>
-  <si>
-    <t>Львівський академічний театр естрадних мініатюр «І люди, і ляльки»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2010/07/teatr-i-liudy-i-lialky-logo.jpg</t>
-  </si>
-  <si>
-    <t>Репертуар вистав Львівського театру естрадних мініатюр «І люди, і ляльки» на вересень 2019 року</t>
-  </si>
-  <si>
-    <t>Львівський академічний обласний театр ляльок. Репертуар на вересень 2019</t>
-  </si>
-  <si>
-    <t>Львівський академічний обласний театр ляльок</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2010/07/lvivskyi-akademicnyi-oblasnyi-teatr-lalok.jpg</t>
-  </si>
-  <si>
-    <t>Репертуар вистав Львівського академічного обласного театру ляльок на вересень 2019 року</t>
-  </si>
-  <si>
-    <t>Гурт «Без Обмежень» презентує нову програму</t>
-  </si>
-  <si>
-    <t>2019-10-01T17:00, 20:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-bez-obmezhen-new.jpg</t>
-  </si>
-  <si>
-    <t>Найліричніший рок-гурт України «Без Обмежень» представить нову програму. Вже в серпні на українців чекає новий альбом гурту, а поки що хлопці вирішили потішити шанувальників новим синглом «Мільярди». Це пісня про нестримну силу кохання, про подолання відстані</t>
-  </si>
-  <si>
-    <t>Фестиваль аудіовізуального мистецтва «Тетраматика 2019»</t>
-  </si>
-  <si>
-    <t>2019-10-04</t>
-  </si>
-  <si>
-    <t>Різні локації міста</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-tetramatyka-2019.jpg</t>
-  </si>
-  <si>
-    <t>Цьогоріч програма складається з кількох мистецьких блоків: експозиції «Human aspect: on/off», виставки «Time forward, two times back / Dot.to.dot», серії аудіовізуальних проектів «+100» та конференції «Digital Cultures»</t>
-  </si>
-  <si>
-    <t>8 Перегляд сучасного польського кіно «Під Високим Замком»</t>
-  </si>
-  <si>
-    <t>КІНО</t>
-  </si>
-  <si>
-    <t>Кінотеатр «Кінопалац»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-PNFP-2019.jpg</t>
-  </si>
-  <si>
-    <t>Світ навколо нас динамічно змінюється, надходять несподівані звістки і нечувані події, неймовірні відкриття і неочікувані явища. Тільки Перегляд щороку пропонує одне й те ж – найкращі і найновіші польські фільми</t>
-  </si>
-  <si>
-    <t>Концерт гурту «Лісапетний батальйон»</t>
-  </si>
-  <si>
-    <t>2019-10-04T19:00</t>
-  </si>
-  <si>
-    <t>Львівський державний цирк</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2017/03/afisha-lisapetnyi-batalion.jpg</t>
-  </si>
-  <si>
-    <t>До вашої уваги дві години сміхотерапії, нові пісні та улюблені хіти, подарунки для глядачів, а також народне камеді-шоу від Наталії Фаліон. Звучатимуть і вже відомі пісні, які принесли колективу перемогу на талант-шоу, і новинки</t>
-  </si>
-  <si>
-    <t>Концерт гурту «Лісапетний батальйон» на Сихові</t>
-  </si>
-  <si>
-    <t>2019-10-05T16:00</t>
-  </si>
-  <si>
-    <t>Центр Довженка</t>
-  </si>
-  <si>
-    <t>«Лісапетний батальйон» – найяскравіший приклад того, як зірки з народу пробиваються на вершину слави. 25 років колектив прикольних і веселих жінок йшов до настільки серйозного концерту</t>
-  </si>
-  <si>
-    <t>Концерт Володимира Окілко «Ювілейний»</t>
-  </si>
-  <si>
-    <t>2019-10-06T17:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-volodymyr-okilko.jpg</t>
-  </si>
-  <si>
-    <t>Під час виступу Окілко виконає пісні які стали улюбленими серед його прихильників, а також нові його твори. У концерті братиме участь неперевершений сатирик та гуморист Гриць Драпак, а також донька Володимира, юна співачка Лідія Окілко - LiDiiA</t>
-  </si>
-  <si>
-    <t>30-ий міжнародний театральний фестиваль «Золотий Лев – 2019»</t>
-  </si>
-  <si>
-    <t>2019-09-28</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-zolotyi-lev-2019.jpg</t>
-  </si>
-  <si>
-    <t>Відкриття фестивалю відбудеться маштабною карнавальною ходою за участю театрів України, Польщі, Чехії, США. Далі впродовж дев’яти днів львів’яни та гості міста зможуть насолоджуватись неймовірним мистецьким дійством на площах Львова та в приміщеннях Львівських театрів</t>
-  </si>
-  <si>
-    <t>Концерт фрік-кабаре Dakh Daughters</t>
-  </si>
-  <si>
-    <t>2019-10-07T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2014/11/afisha-dakh-band.jpg</t>
-  </si>
-  <si>
-    <t>Dakh Daughters. Нова програма. Ті, що закохали в себе Париж! Фрік-кабаре Dakh Daughters Band – це сім талановитих красунь, акторок театру «Дах» Влада Троїцького. Це – п'ятнадцять музичних інструментів, діапазон вокалу від українського плачу до суворого гроулінгу</t>
-  </si>
-  <si>
-    <t>Концерт Lords Of The Sound з програмою «Кінохіти. Краще за 5 років»</t>
-  </si>
-  <si>
-    <t>2019-10-08T20:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-lords-best.jpeg</t>
-  </si>
-  <si>
-    <t>Ювілейний концерт від Lords of the Sound. За цей час музиканти встигли проявити себе в абсолютно різних амплуа, подарувавши нам найрізноманітнішу музику. Вони стали першими впроваджувати запальний формат оркестрових концертів, відходячи від стереотипного академізму</t>
-  </si>
-  <si>
-    <t>Виставка Анни Варшавської Mitosis</t>
-  </si>
-  <si>
-    <t>2019-09-25</t>
-  </si>
-  <si>
-    <t>Галерея Львівської національної академії мистецтв</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-anna-varshavska-mitosis.jpg</t>
-  </si>
-  <si>
-    <t>Персональна виставка Анни Варшавської, що представить серію монументальних графічних творів, виконаних у доволі нетиповій техніці - кульковою ручкою. До експозиції увійдуть великоформатні графічні твори та відеоарт</t>
-  </si>
-  <si>
-    <t>Виставка «Форма збереження»</t>
-  </si>
-  <si>
-    <t>2019-07-16</t>
-  </si>
-  <si>
-    <t>Кафе-вітальня Центру міської історії</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-forma-zberezhennia.jpg</t>
-  </si>
-  <si>
-    <t>Виставка фотографій Танаса Никофорука та Сергія Братковського на яких зафіксовані ґрати - не лише як інструмент фізичного захисту, але й засіб для культивування та збереження власної ідентичності</t>
-  </si>
-  <si>
-    <t>Макс Кідрук презентує роман «Доки світло не згасне назавжди»</t>
-  </si>
-  <si>
-    <t>2019-10-10T19:00</t>
-  </si>
-  <si>
-    <t>ЛІТЕРАТУРА</t>
-  </si>
-  <si>
-    <t>Торгова галерея «Опера Пасаж» / Opera Passage</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-svitlo-Maks-Kidruk.jpg</t>
-  </si>
-  <si>
-    <t>Презентація в рамках всеукраїнського туру письменника Макса Кідрука на підтримку нового роману «Доки світло не згасне назавжди» у Львові</t>
-  </si>
-  <si>
-    <t>Концерт гурту Imprintband</t>
-  </si>
-  <si>
-    <t>2019-10-11T19:00</t>
-  </si>
-  <si>
-    <t>Малевич: night club &amp; concert arena</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/Imprintband.jpg</t>
-  </si>
-  <si>
-    <t>Концерт молодіжного християнського гурту Imprintband – колективу, який любить Бога і справу свого життя – музику. Самі учасники колективу стверджують, що тільки Бог міг об’єднати таких різних, несхожих один на одного, людей. У кожного з них свої мрії, свої пріоритети і погляди на життя, але не дивлячись на відмінності в характері, їх об’єднує неймовірна всеосяжна […]</t>
-  </si>
-  <si>
-    <t>Виставка «Графічні Фантасмагорії»</t>
-  </si>
-  <si>
-    <t>2019-09-13</t>
-  </si>
-  <si>
-    <t>Львівська Мануфактура Кави</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-hrafichni-fantasmahorii.jpg</t>
-  </si>
-  <si>
-    <t>На виставці представлено 30 робіт мисткині ERA Khelovneba із циклу «Світ мого маленького світу», створених у період від 2001 року (більшість робіт 2014 – 2018 років)</t>
-  </si>
-  <si>
-    <t>Конгрес культури «Перехід 1989»</t>
-  </si>
-  <si>
-    <t>2019-10-11</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/06/afisha-kongres-kultury-perehid.png</t>
-  </si>
-  <si>
-    <t>Перший конгрес — «Перехід 1989» — хронологічно та метафорично відштовхується від 1989 року. Він матиме три тематичні блоки, в рамках яких відбуватимуться дискусії: Мури. Міри. Наміри. Учасники конгресу спробують спільно означити, як і що змінилося у культурній ситуації незалежної України</t>
-  </si>
-  <si>
-    <t>Вистава «Королева краси»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2018/05/afisha-koroleva-krasy.jpg</t>
-  </si>
-  <si>
-    <t>Тема периферійної, ізольованої людини, яка прагне омріяного життя, але не в змозі його досягнути. Через страхи минулого, що переносяться на реальність, нездатність реалізовувати свої мрії, це бажане життя залишається непрожитим</t>
-  </si>
-  <si>
-    <t>Екскурсія «Софіївка + Шевченкове + Вінницький фонтан»</t>
-  </si>
-  <si>
-    <t>ЕКСКУРСІЇ ЗА МІСТО</t>
-  </si>
-  <si>
-    <t>Львів – Моринці-Шевченкове – Національний дендропарк «Софіївка» – Вінниця – Меджибіж – Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2013/05/Sofiyivka.jpg</t>
-  </si>
-  <si>
-    <t>Запрошуємо пройтися місцями Великого Кобзаря, побачити красу та фортеці Поділля, пейзажі Південного Бугу та оглянути один з красивіших парків України. Тривалість туру - 2 дні та 2 ночі</t>
-  </si>
-  <si>
-    <t>Екскурсія «Тунель кохання, форт війни та замок»</t>
-  </si>
-  <si>
-    <t>2019-10-12</t>
-  </si>
-  <si>
-    <t>Львів - Клевань (Тунель кохання) - Тараканів (форт) - Дубно (замок) - Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2013/05/Klevan-tunel1.jpg</t>
-  </si>
-  <si>
-    <t>Мандрівка до створеного природою Тунелі кохання у Клевані, відвідування чудо інженерної військової думки - Тараканівсього форту та нездоланного Дубненського замку. Тривалість туру - 1 день</t>
-  </si>
-  <si>
-    <t>Виставка «Обабіч»</t>
-  </si>
-  <si>
-    <t>2019-09-22</t>
-  </si>
-  <si>
-    <t>Lem Station</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-obabich.jpg</t>
-  </si>
-  <si>
-    <t>Три актуальні, але різні реальності сучасної України, існують обабіч одна одної, паралельно в просторі, але не завжди в одному часі. Що спільного в людей, які творять ці реальності? Що їх об’єднує?</t>
-  </si>
-  <si>
-    <t>Концерт Івана Поповича</t>
-  </si>
-  <si>
-    <t>2019-10-13T16:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2011/10/ivan-popovych.jpeg</t>
-  </si>
-  <si>
-    <t>Народний артист України Іван Попович представить свою нову програму «Трембітар української душі», однойменна пісня якій присвячена пам’яті Степана Бандери</t>
-  </si>
-  <si>
-    <t>Вистава «Пригоди італійців в Італії»</t>
-  </si>
-  <si>
-    <t>2019-10-14T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-prygody-italijciv.jpg</t>
-  </si>
-  <si>
-    <t>Прем'єра дивовижної комедії на італійський лад. Нестримний сміх, цікавий сюжет і зіркові актори українського театру і кінематографу: Руслана Писанка, Олексій Вертинський, Лесь Задніпровський</t>
-  </si>
-  <si>
-    <t>Екскурсія «Озеро Синевир та водоспад Шипіт»</t>
-  </si>
-  <si>
-    <t>2019-10-14</t>
-  </si>
-  <si>
-    <t>Львів – водоспад Шипіт – Синевирський перевал – озеро Синевир – Келечин – Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2014/07/ozero-synevyr.jpg</t>
-  </si>
-  <si>
-    <t>Синевирський перевал, реабілітаційний центр бурого ведмедя, озеро Синевир, водоспад Шипіт, дегустація унікальної мінеральної води в Келечині. Тривалість туру - 1 день</t>
-  </si>
-  <si>
-    <t>Виставка Єви Гриник «Гордість міста»</t>
-  </si>
-  <si>
-    <t>2019-09-17</t>
-  </si>
-  <si>
-    <t>Будинок органної та камерної музики</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-vystavka-hordist-mista.jpg</t>
-  </si>
-  <si>
-    <t>Ви, напевно, бачили ці мальовані плакати на сітілайтах Львова. Видатні львів’яни, які прославили наше місто. Люди різних професій, національностей, поглядів. Вони ходили вулицями Львова в різні часи, але всі залишилися в його пам’яті</t>
-  </si>
-  <si>
-    <t>Вистава «Апокрифи»</t>
-  </si>
-  <si>
-    <t>2019-10-18T19:00</t>
-  </si>
-  <si>
-    <t>Це низка історій, об'єднаних темою. Підкреслюється одна лінія. Звичайно, при такій побудові детальна розробка нюансів, психологізм образів змінюється виділенням якоїсь однієї риси.</t>
-  </si>
-  <si>
-    <t>Екскурсія-тур «Сиро-Винний тур Закарпаттям»</t>
-  </si>
-  <si>
-    <t>2019-10-19</t>
-  </si>
-  <si>
-    <t>Львів – палац Шенборна – Мукачево – Берегово – Нижнє Селище – озеро Синевир – водоспад Шипіт – Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2013/01/afisha_Syro_Vynnyy_tur_Zakarpattyam.jpg</t>
-  </si>
-  <si>
-    <t>Палац Шенборна, Мукачівський замок, басейн в Берегово, дегустації вина та сиру, водоспат Шипіт та озеро Синевир - все найкраще у Закарпатті. Тривалість туру - 2 дні</t>
-  </si>
-  <si>
-    <t>Вистава «Забави для Фауста»</t>
-  </si>
-  <si>
-    <t>2019-10-19T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2010/05/afisha_zabavy_dya_fausta.png</t>
-  </si>
-  <si>
-    <t>«Забави для Фауста» — забави вишукані та витончені, де чорно-золотий Свидригайлов бавиться з ляльками</t>
-  </si>
-  <si>
-    <t>Виставка Богдана Сороки «Графіка»</t>
-  </si>
-  <si>
-    <t>2019-09-24</t>
-  </si>
-  <si>
-    <t>Мистецька галерея «Зелена Канапа»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-bohgan-soroka.jpg</t>
-  </si>
-  <si>
-    <t>Богдан Сорока – видатний художник-графік, дисидент, що причетний до творення сучасного мистецтва України ХХ століття. В експозиції буде представлено роботи з кількох серій кольорових та чорно-білих ліноритів, багато з яких будуть виставлятися вперше</t>
-  </si>
-  <si>
-    <t>Виставка Ігоря Яновича «Чорне»</t>
-  </si>
-  <si>
-    <t>2019-09-10</t>
-  </si>
-  <si>
-    <t>Арт-центр Павла Гудімова «Я Галерея. Львів»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-yanovych-chorne.jpg</t>
-  </si>
-  <si>
-    <t>Виставка Ігоря Яновича є достатньо особистою, щоб глядач/ка могли потрапити у суб'єктивний простір автора і відчути власні переживання, але й більшою за окремий досвід, адже виходить на ширше визначальне питання: що таке досвід споглядання, коли діє чорне?</t>
-  </si>
-  <si>
-    <t>Виставка творів Марії Примаченко</t>
-  </si>
-  <si>
-    <t>2019-09-03</t>
-  </si>
-  <si>
-    <t>Українське мистецтво ХХ ст. Відділ НМЛ ім. Андрея Шептицького</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-maria-prymachenko.jpg</t>
-  </si>
-  <si>
-    <t>Виставка творів яскравої представниці «наївного» мистецтва Марії Примаченко. Понад шістдесят робіт із приватної колекції (Київ) та зі збірки Національного музею у Львові ім. Андрея Шептицького репрезентують її мистецький спадок 1960–1990-х років</t>
-  </si>
-  <si>
-    <t>Вистава «Маркіза de Sade»</t>
-  </si>
-  <si>
-    <t>2019-10-20T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/05/afisha-vystava-markiza-de-sade.jpg</t>
-  </si>
-  <si>
-    <t>Чи справді жорстокість є невід’ємною частиною природи людини, а темні бажання керують її вчинками? Чи можна прийняти твердження, що гріх та надмірність ведуть до очищення і звільнення?</t>
-  </si>
-  <si>
-    <t>Акустичний концерт гурту The Hardkiss</t>
-  </si>
-  <si>
-    <t>2019-10-21T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/04/afisha-The-Hardkiss-acustic.jpg</t>
-  </si>
-  <si>
-    <t>Особлива атмосфера, понад п’ятнадцяти музикантів-мультиінструменталістів на сцені та головні пісні гурту The Hardkiss в новому звучанні. Головні хіти гурту пролунають в несподіваних аранжуваннях в акустиці завдяки класичним та народним інструментам</t>
+    <t>Музична казка для дітей і дорослих «Лис Микита» – насичена, яскрава та приправлена гумором казка про звірів. Опера на 2 дії, музика Івана Небесного, лібрето Василя Вовкуна за однойменною поемою Івана Франка де він зобразив людські натури заховавши їх за масками тварин</t>
+  </si>
+  <si>
+    <t>Виставка Марії Пляцко й Олександри Сиси «Форма»</t>
+  </si>
+  <si>
+    <t>Галерея сучасного сакрального мистецтва «IconArt»</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/11/afisha-pliacko-sysa-forma.jpg</t>
+  </si>
+  <si>
+    <t>Простір рухливий, мінливий. Його форму ми споживаємо й переживаємо повсякденно, перебудовуємо, руйнуємо, змінюємо, переплановуємо під себе. Канву простору, з її об’єктами та рухливим формотворенням, створюємо ми, але водночас ми є її елементами</t>
+  </si>
+  <si>
+    <t>Вистава Timetravellers</t>
+  </si>
+  <si>
+    <t>2019-12-15T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2019/05/afisha-vystava-timetravellers.jpg</t>
+  </si>
+  <si>
+    <t>На Донбасі є великий пам’ятник Артему, якого насправді звали Федір. Це парадокс. Їх не уникнути. Ви зрозумієте це, коли буде занадто пізно. Вишні і абрикоси все одно цвістимуть, а зірки світитимуть</t>
+  </si>
+  <si>
+    <t>Орекстр K&amp;K Philharmoniker: Віденський Йоганна Штрауса Концерт–Гала</t>
+  </si>
+  <si>
+    <t>2019-12-17T19:00</t>
+  </si>
+  <si>
+    <t>Львівська обласна філармонія</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2014/11/afisha_Philharmoniker-.jpeg</t>
+  </si>
+  <si>
+    <t>Симфонічний оркестр K&amp;K Philharmoniker під керівництвом австрійського композитора та диригента Маттіаса Георга Кендлінгера презентують надзвичайно мелодійні, невимушені та енергійні композиції з характерним стилем композиторської династії Штраусів</t>
+  </si>
+  <si>
+    <t>Вистава «Варшавська мелодія»</t>
+  </si>
+  <si>
+    <t>2019-12-17T18:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2009/11/afisha_varshavska_melodiya.jpg</t>
+  </si>
+  <si>
+    <t>П'єса «Варшавська мелодія» написана Леонідом Зоріном в 1967 році - саме тоді, коли дозволений був дещо вільніший погляд на світ і можна було критикувати окремі недоліки сталінського керівництва.</t>
   </si>
   <si>
     <t>Вистава «Ножі в курях, або Спадок мірошника»</t>
   </si>
   <si>
-    <t>2019-10-23T19:00</t>
+    <t>2019-12-18T19:00</t>
   </si>
   <si>
     <t>https://lviv-online.com/ua/wp-content/uploads/2016/02/afisha-vystava-nozhi-v-kuriakh.jpg</t>
@@ -581,301 +485,160 @@
     <t>Вистава за п'єсою сучасного шотландського драматурга Девіда Гарровера «Ножі в курях»</t>
   </si>
   <si>
-    <t>Екскурсія-тур «10 родзинок Закарпаття»</t>
-  </si>
-  <si>
-    <t>2019-10-25</t>
-  </si>
-  <si>
-    <t>Львів - палац Шенборна - Мукачево - Берегово - Ужгород - Лумшори - Іза - озеро Синевир - водоспад Шипіт - Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2014/04/Nevycke.jpg</t>
-  </si>
-  <si>
-    <t>Карпати, замки, палаци, вина, все найкраще, що може запропонувати гостинне Закарпаття, чекає на Вас. Тривалість туру - 3 дні</t>
-  </si>
-  <si>
-    <t>Вистава «Лісова пісня»</t>
-  </si>
-  <si>
-    <t>2019-10-25T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2011/02/afisha_lisova_pisnya_kurbasa.jpg</t>
-  </si>
-  <si>
-    <t>Вистава за п'єсою Лесі Українки у трьох колядах (за підтримки Благодійного Фонду «Розвиток України»). У виставі використані пісні фольклорних гуртів «Кросна», «Божичі», «Древо».</t>
-  </si>
-  <si>
-    <t>Екскурсія-тур «Сплав по Черемошу і не лише»</t>
-  </si>
-  <si>
-    <t>2019-10-26</t>
-  </si>
-  <si>
-    <t>Львів – Рогатин – Яремче – Буковель – Поляниця – сплав річкою Чорний Черемош – Верховина – Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2015/09/splav.jpg</t>
-  </si>
-  <si>
-    <t>Чудова нагода активно відпочити та подихати чистим повітрям. Огляд водоспаду у Яремче, церква у Рогатині, канатно-крісельна дорога на Буковель та справ річкою Чорний Черемош. Тривалість туру - 2 дні</t>
-  </si>
-  <si>
-    <t>Екскурсія-тур «Яремче, Буковель + Говерла»</t>
-  </si>
-  <si>
-    <t>Львів – Рогатин – Яремче – Буковель – Поляниця – сходження на Говерлу – Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2015/09/goverla.jpg</t>
-  </si>
-  <si>
-    <t>Запрошуємо піднятися на найвищу вершину в Україні, а також побачити фантастичні гірські пейзажі та водоспади. Тривалість туру - 2 дні</t>
-  </si>
-  <si>
-    <t>Вистава «Формули екстази»</t>
-  </si>
-  <si>
-    <t>2019-10-26T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2009/10/antonych_formuly.jpg</t>
-  </si>
-  <si>
-    <t>Вистава «Формули екстази» є драматичними замальовками за текстами Богдана Ігоря Антонича та Луїджі Піранделло. Режисером вистави є Олег Цьона.</t>
-  </si>
-  <si>
-    <t>Концерт гурту The Rasmus</t>
-  </si>
-  <si>
-    <t>2019-10-27T20:00</t>
-  </si>
-  <si>
-    <t>Стадіон «Арена Львів»</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/04/afisha-The-Rasmus.jpg</t>
-  </si>
-  <si>
-    <t>Чорний одяг, мейк-ап, пісня «In the Shadows» в навушниках. Відчули приємну ностальгію? Найвідоміша група Фінляндії: дев’ять студійних альбомів, величезна кількість музичних нагород, любов армії шанувальників і культовий статус в історії рок-музики нульових</t>
-  </si>
-  <si>
-    <t>Вистава «Так казав Заратустра»</t>
-  </si>
-  <si>
-    <t>2019-10-27T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2012/12/afisha_tak_kazav_zaratustra.jpg</t>
-  </si>
-  <si>
-    <t>Проект орієнтовано насамперед на пошук духовних джерел, драйву життя через форми слова, пластики, співу, візуального оформлення. Спроба перенести думки Ніцше/Заратустри у сьогоднішні українські реалії</t>
-  </si>
-  <si>
-    <t>Музично-танцювальне шоу Ladies Night</t>
-  </si>
-  <si>
-    <t>2019-10-29T20:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-ladysnight.jpg</t>
-  </si>
-  <si>
-    <t>Крихітне провінційне містечко у Великобританії. Довгий час єдиним роботодавцем для жителів був металургійний комбінат, але він закрився. Історія розповість про шістьох друзів, які зайняті пошуком роботи. Учасники: актор Антон Лірник, шоумен Олександр Педан, танцюрист Влад Яма, співак Арсен Мірзоян</t>
-  </si>
-  <si>
-    <t>Виставка «Мистецтво войовничого плакату»</t>
-  </si>
-  <si>
-    <t>Львівський історичний музей. Відділ «Кам’яниця Корнякта» / Італійське подвір’я</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-mystetstvo-voiovnychoho-pakatu.jpg</t>
-  </si>
-  <si>
-    <t>На виставці у Львівському історичному музеї представлено 53 художні плакати (російські, німецькі, англійські, радянські, австрійські, українські, польські), які дають можливість побачити як змінювався художній стиль, образотворчі метафори, символи, характер шрифту, техніка виконання плакату</t>
-  </si>
-  <si>
-    <t>Триб’ют-шоу Адріано Челентано</t>
-  </si>
-  <si>
-    <t>2019-11-05T20:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-chelentano-tribut.jpg</t>
-  </si>
-  <si>
-    <t>Творча спадщина легенди італійського кіно і музики Адріано Челентано в унікальному триб'ют-шоу «Lui e gli amici del Re». На сцені неперевершений імітатор - маестро Адольфо Себастьяні. Захоплююча атмосфера, яка панувала на незабутніх концертах великого Артиста</t>
-  </si>
-  <si>
-    <t>Виставка «Адам Смоляна / Львів 1921 – Сопот 1987»</t>
-  </si>
-  <si>
-    <t>2019-09-19</t>
-  </si>
-  <si>
-    <t>Музей Івана Георгія Пінзеля</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/09/afisha-adam-smoliana.jpg</t>
-  </si>
-  <si>
-    <t>Виставка робіт Адама Смоляни – митця, чиї роботи пов’язують з досягненнями так званої Сопотської школи (зараз Академія образотворчих мистецтв у Гданську). Окрім скульптур – переважно з дерева – в експозиції будуть представлені роботи з гіпсу, металу, а також графіка</t>
-  </si>
-  <si>
-    <t>Оксана Муха з програмою «Найгарніші пісні України»</t>
-  </si>
-  <si>
-    <t>2019-11-11T20:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-oksanamuha.jpg</t>
-  </si>
-  <si>
-    <t>Сольний концерт співачки, скрипальки, переможниці дев‘ятого сезону популярного телепроекту «Голос країни», заслуженої артистки України Оксани Мухи у рідному Львові! З новою концертною програмою «Найгарніші пісні України» — у супроводі оркестру і рок-бенду</t>
-  </si>
-  <si>
-    <t>Екскурсія-тур «Золота Підкова + Замок мушкетерів»</t>
-  </si>
-  <si>
-    <t>2019-11-16</t>
-  </si>
-  <si>
-    <t>Підгорецький, Олеський, Золочівський та Свіржський замки</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2015/10/Olesko-zamok.jpg</t>
-  </si>
-  <si>
-    <t>Запрошуємо Вас оглянути чотири мальовничі замки Львівщини: Підгорецький, Олеський, Золочівський та Свіржський. Тривалість туру - 1 день</t>
-  </si>
-  <si>
-    <t>Релакс-тур «Термальне Закарпаття»</t>
-  </si>
-  <si>
-    <t>Львів – Чинадієво – Мукачево – Берегівське вулканічне низькогір’я – Ужгород – Лумшори – Львів</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2015/02/zymove-kosyno-tur.jpg</t>
-  </si>
-  <si>
-    <t>Замок Сент-Міклош у Чинадієво, купання в термальних басейнах Косино та в лумшорських чанах, дегустація вин Берегівщини, центр та замок в Ужгороді. Тривалість туру - 2 дні</t>
-  </si>
-  <si>
-    <t>Гурт Oomph! презентує альбом Ritual</t>
-  </si>
-  <si>
-    <t>2019-11-17T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/04/afisha-Oomph.jpg</t>
-  </si>
-  <si>
-    <t>Ritual - перша за чотири роки платівка в дискографії Oomph! Будучи піонерами танцювального металу, Oomph! в цій роботі вирішили повернутися до свого коріння, тільки зробивши звучання набагато важче, ніж раніше</t>
-  </si>
-  <si>
-    <t>Ювілейний концерт Степана Гіги</t>
-  </si>
-  <si>
-    <t>2019-11-18T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2012/02/afisha-uvileinyi-giga.jpg</t>
-  </si>
-  <si>
-    <t>Мабуть, на українській естраді важко знайти виконавця, який завойовує серця аудиторії з першого акорду пісні чи першої строфи тексту. Степан Гіга ось уже понад чверть століття впевнено займає лідерські позиції на варті української пісні</t>
-  </si>
-  <si>
-    <t>«Бумбокс» презентує альбом «Таємний код»</t>
-  </si>
-  <si>
-    <t>2019-11-22T19:00</t>
-  </si>
-  <si>
-    <t>https://lviv-online.com/ua/wp-content/uploads/2019/07/afisha-bumboks-taemnyi-kod.jpg</t>
-  </si>
-  <si>
-    <t>В процесі створення альбому з групи пішли гітарист і басист. Альбом «Таємний код» скдається з двох частин, в якому вперше за 15 років існування гурту «Бумбокс» буде більше 11 пісень. Три з них добре тобі знайомі і стали суперхітами</t>
-  </si>
-  <si>
-    <t>2019-09-30 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-01 17:00, 20:00</t>
-  </si>
-  <si>
-    <t>2019-10-04 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-05 16:00</t>
-  </si>
-  <si>
-    <t>2019-10-06 17:00</t>
-  </si>
-  <si>
-    <t>2019-10-07 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-08 20:00</t>
-  </si>
-  <si>
-    <t>2019-10-10 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-11 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-13 16:00</t>
-  </si>
-  <si>
-    <t>2019-10-14 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-18 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-19 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-20 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-21 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-23 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-25 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-26 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-27 20:00</t>
-  </si>
-  <si>
-    <t>2019-10-27 19:00</t>
-  </si>
-  <si>
-    <t>2019-10-29 20:00</t>
-  </si>
-  <si>
-    <t>2019-11-05 20:00</t>
-  </si>
-  <si>
-    <t>2019-11-11 20:00</t>
-  </si>
-  <si>
-    <t>2019-11-17 19:00</t>
-  </si>
-  <si>
-    <t>2019-11-18 19:00</t>
-  </si>
-  <si>
-    <t>2019-11-22 19:00</t>
+    <t>Вистава «Стежечка святого Миколая»</t>
+  </si>
+  <si>
+    <t>2019-12-19T11:00, 14:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2013/12/afisha-stezhechka-sviatogo-mykolaia.jpeg</t>
+  </si>
+  <si>
+    <t>Для того, аби Миколай спустився з небес, зірки вказують йому шлях на землю. Чи ж зможе дістатися до нас Миколай, якщо хитрий Чорт, змовившись із Вовком, сховає зірки?</t>
+  </si>
+  <si>
+    <t>Опера «Наталка Полтавка»</t>
+  </si>
+  <si>
+    <t>2019-12-19T18:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2009/12/opera-natalka-poltavka.jpg</t>
+  </si>
+  <si>
+    <t>Класична історія про любов і вірність за пєсою, з якої починався український театр на початку ХІХ століття. Її знає тепер кожен школяр, але не кожен слухав народні мелодії в обробці Лисенка</t>
+  </si>
+  <si>
+    <t>Вистава «Перехресні стежки»</t>
+  </si>
+  <si>
+    <t>2019-12-20T19:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2018/12/afisha-perekhresni-stezhky.jpg</t>
+  </si>
+  <si>
+    <t>«Перехресні стежки» – це перегук часів, минулого (Франкового) і нашого теперішнього (ХХІ століття) через розкриття психологічної та соціальної драми. Історичний фон для таких дієвих пошуків може змінюватись, але незмінною лишається внутрішня драма особистості</t>
+  </si>
+  <si>
+    <t>Вистава-забава «Миколай прийшов до нас»</t>
+  </si>
+  <si>
+    <t>2019-12-20T11:00, 13:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2014/12/afisha-mykolai-pryishov-do-nas.jpeg</t>
+  </si>
+  <si>
+    <t>Львівський академічний духовний театр «Воскресіння» запрошує всіх зустрітися зі святим Миколаєм в Довженко-центрі. Надзвичайно цікава, як діткам, так і дорослим вистава-забава</t>
+  </si>
+  <si>
+    <t>Опера «Севільський цирульник»</t>
+  </si>
+  <si>
+    <t>2019-12-20T18:00</t>
+  </si>
+  <si>
+    <t>https://lviv-online.com/ua/wp-content/uploads/2010/10/opera-sevilskyi-tserulnyk.jpg</t>
+  </si>
+  <si>
+    <t>Нічну тишу однієї з вулиць Севільї порушує серенада. Це граф Альмавіва, який видає себе за бідного юнака Ліндора, розповідає про своє кохання до красуні Розіни</t>
+  </si>
+  <si>
+    <t>2019-12-06 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-06 12:00</t>
+  </si>
+  <si>
+    <t>2019-12-06 13:00</t>
+  </si>
+  <si>
+    <t>2019-12-07 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-07 17:00</t>
+  </si>
+  <si>
+    <t>2019-12-07 12:00, 14:00</t>
+  </si>
+  <si>
+    <t>2019-12-07 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-08 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-08 12:00, 14:00, 16:00</t>
+  </si>
+  <si>
+    <t>2019-12-08 12:00</t>
+  </si>
+  <si>
+    <t>2019-12-10 12:00</t>
+  </si>
+  <si>
+    <t>2019-12-11 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-11 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-12 13:00</t>
+  </si>
+  <si>
+    <t>2019-12-12 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-13 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-13 12:00</t>
+  </si>
+  <si>
+    <t>2019-12-13 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-14 13:00</t>
+  </si>
+  <si>
+    <t>2019-12-14 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-14 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-14 12:00, 14:00</t>
+  </si>
+  <si>
+    <t>2019-12-15 12:00, 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-15 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-17 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-17 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-18 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-19 11:00, 14:00</t>
+  </si>
+  <si>
+    <t>2019-12-19 18:00</t>
+  </si>
+  <si>
+    <t>2019-12-20 19:00</t>
+  </si>
+  <si>
+    <t>2019-12-20 11:00, 13:00</t>
+  </si>
+  <si>
+    <t>2019-12-20 18:00</t>
   </si>
 </sst>
 </file>
@@ -955,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="371">
+  <cellXfs count="491">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
       <alignment horizontal="left"/>
@@ -975,6 +738,366 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true">
       <alignment horizontal="left"/>
     </xf>
@@ -2070,11 +2193,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="80.90625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.9453125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="19.6953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="108.6484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="92.57421875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="110.5546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="29.0390625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.77734375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="85.0078125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="91.67578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2103,7 +2226,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s" s="12">
-        <v>7</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s" s="13">
         <v>8</v>
@@ -2123,7 +2246,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s" s="18">
-        <v>261</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s" s="19">
         <v>14</v>
@@ -2143,33 +2266,33 @@
         <v>18</v>
       </c>
       <c r="B4" t="s" s="24">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s" s="25">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s" s="26">
         <v>20</v>
       </c>
-      <c r="D4" t="s" s="26">
+      <c r="E4" t="s" s="27">
         <v>21</v>
       </c>
-      <c r="E4" t="s" s="27">
+      <c r="F4" t="s" s="28">
         <v>22</v>
-      </c>
-      <c r="F4" t="s" s="28">
-        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="29">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s" s="30">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s" s="31">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s" s="32">
         <v>25</v>
-      </c>
-      <c r="D5" t="s" s="32">
-        <v>15</v>
       </c>
       <c r="E5" t="s" s="33">
         <v>26</v>
@@ -2183,13 +2306,13 @@
         <v>28</v>
       </c>
       <c r="B6" t="s" s="36">
-        <v>7</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s" s="37">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s" s="38">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s" s="39">
         <v>30</v>
@@ -2203,10 +2326,10 @@
         <v>32</v>
       </c>
       <c r="B7" t="s" s="42">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="C7" t="s" s="43">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s" s="44">
         <v>33</v>
@@ -2223,13 +2346,13 @@
         <v>36</v>
       </c>
       <c r="B8" t="s" s="48">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s" s="49">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s" s="50">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s" s="51">
         <v>38</v>
@@ -2243,233 +2366,233 @@
         <v>40</v>
       </c>
       <c r="B9" t="s" s="54">
-        <v>7</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s" s="55">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s" s="56">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s" s="57">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s" s="58">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="59">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s" s="60">
-        <v>262</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s" s="61">
         <v>14</v>
       </c>
       <c r="D10" t="s" s="62">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s" s="63">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s" s="64">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="65">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s" s="66">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s" s="67">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s" s="68">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s" s="69">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s" s="70">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="71">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s" s="72">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s" s="73">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s" s="74">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s" s="75">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s" s="76">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="77">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s" s="78">
-        <v>263</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s" s="79">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s" s="80">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s" s="81">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s" s="82">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="83">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s" s="84">
-        <v>264</v>
+        <v>184</v>
       </c>
       <c r="C14" t="s" s="85">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s" s="86">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s" s="87">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s" s="88">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="89">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s" s="90">
-        <v>265</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s" s="91">
         <v>14</v>
       </c>
       <c r="D15" t="s" s="92">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s" s="93">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s" s="94">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="95">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s" s="96">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s" s="97">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s" s="98">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s" s="99">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s" s="100">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="101">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s" s="102">
-        <v>266</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s" s="103">
         <v>14</v>
       </c>
       <c r="D17" t="s" s="104">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s" s="105">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s" s="106">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="107">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s" s="108">
-        <v>267</v>
+        <v>188</v>
       </c>
       <c r="C18" t="s" s="109">
         <v>14</v>
       </c>
       <c r="D18" t="s" s="110">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s" s="111">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F18" t="s" s="112">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="113">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s" s="114">
-        <v>84</v>
+        <v>189</v>
       </c>
       <c r="C19" t="s" s="115">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s" s="116">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s" s="117">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s" s="118">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="119">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s" s="120">
-        <v>89</v>
+        <v>190</v>
       </c>
       <c r="C20" t="s" s="121">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s" s="122">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s" s="123">
         <v>91</v>
@@ -2483,413 +2606,413 @@
         <v>93</v>
       </c>
       <c r="B21" t="s" s="126">
-        <v>268</v>
+        <v>191</v>
       </c>
       <c r="C21" t="s" s="127">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s" s="128">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s" s="129">
         <v>95</v>
       </c>
-      <c r="D21" t="s" s="128">
+      <c r="F21" t="s" s="130">
         <v>96</v>
-      </c>
-      <c r="E21" t="s" s="129">
-        <v>97</v>
-      </c>
-      <c r="F21" t="s" s="130">
-        <v>98</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="131">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s" s="132">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="C22" t="s" s="133">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s" s="134">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s" s="135">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="F22" t="s" s="136">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="137">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s" s="138">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="C23" t="s" s="139">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s" s="140">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E23" t="s" s="141">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="F23" t="s" s="142">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="143">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s" s="144">
-        <v>268</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s" s="145">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s" s="146">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s" s="147">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="F24" t="s" s="148">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="149">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s" s="150">
-        <v>269</v>
+        <v>192</v>
       </c>
       <c r="C25" t="s" s="151">
         <v>14</v>
       </c>
       <c r="D25" t="s" s="152">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s" s="153">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F25" t="s" s="154">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="155">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s" s="156">
-        <v>105</v>
+        <v>191</v>
       </c>
       <c r="C26" t="s" s="157">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s" s="158">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s" s="159">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F26" t="s" s="160">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="161">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s" s="162">
-        <v>110</v>
+        <v>194</v>
       </c>
       <c r="C27" t="s" s="163">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s" s="164">
         <v>20</v>
       </c>
-      <c r="D27" t="s" s="164">
-        <v>50</v>
-      </c>
       <c r="E27" t="s" s="165">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F27" t="s" s="166">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="167">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s" s="168">
-        <v>269</v>
+        <v>195</v>
       </c>
       <c r="C28" t="s" s="169">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s" s="170">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s" s="171">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F28" t="s" s="172">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="173">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s" s="174">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s" s="175">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s" s="176">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s" s="177">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="F29" t="s" s="178">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="179">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B30" t="s" s="180">
-        <v>122</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s" s="181">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s" s="182">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s" s="183">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F30" t="s" s="184">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="185">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s" s="186">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="C31" t="s" s="187">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s" s="188">
-        <v>128</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s" s="189">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F31" t="s" s="190">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="191">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s" s="192">
-        <v>270</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s" s="193">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s" s="194">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="E32" t="s" s="195">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F32" t="s" s="196">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="197">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B33" t="s" s="198">
-        <v>271</v>
+        <v>199</v>
       </c>
       <c r="C33" t="s" s="199">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s" s="200">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="E33" t="s" s="201">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F33" t="s" s="202">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="203">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s" s="204">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s" s="205">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s" s="206">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E34" t="s" s="207">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F34" t="s" s="208">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="209">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s" s="210">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="C35" t="s" s="211">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D35" t="s" s="212">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="E35" t="s" s="213">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F35" t="s" s="214">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="215">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s" s="216">
-        <v>272</v>
+        <v>202</v>
       </c>
       <c r="C36" t="s" s="217">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D36" t="s" s="218">
         <v>33</v>
       </c>
       <c r="E36" t="s" s="219">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="F36" t="s" s="220">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="221">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B37" t="s" s="222">
-        <v>153</v>
+        <v>203</v>
       </c>
       <c r="C37" t="s" s="223">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s" s="224">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s" s="225">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F37" t="s" s="226">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="227">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B38" t="s" s="228">
-        <v>273</v>
+        <v>204</v>
       </c>
       <c r="C38" t="s" s="229">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s" s="230">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s" s="231">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F38" t="s" s="232">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="233">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B39" t="s" s="234">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="C39" t="s" s="235">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s" s="236">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s" s="237">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F39" t="s" s="238">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="239">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B40" t="s" s="240">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="C40" t="s" s="241">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s" s="242">
-        <v>168</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s" s="243">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F40" t="s" s="244">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="245">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B41" t="s" s="246">
-        <v>172</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s" s="247">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D41" t="s" s="248">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="E41" t="s" s="249">
         <v>174</v>
@@ -2900,402 +3023,802 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="251">
-        <v>176</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s" s="252">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="C42" t="s" s="253">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D42" t="s" s="254">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E42" t="s" s="255">
-        <v>178</v>
+        <v>99</v>
       </c>
       <c r="F42" t="s" s="256">
-        <v>179</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="257">
-        <v>180</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s" s="258">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="C43" t="s" s="259">
         <v>14</v>
       </c>
       <c r="D43" t="s" s="260">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="E43" t="s" s="261">
-        <v>182</v>
+        <v>104</v>
       </c>
       <c r="F43" t="s" s="262">
-        <v>183</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="263">
-        <v>184</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s" s="264">
-        <v>276</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s" s="265">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D44" t="s" s="266">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="E44" t="s" s="267">
-        <v>186</v>
+        <v>107</v>
       </c>
       <c r="F44" t="s" s="268">
-        <v>187</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="269">
-        <v>188</v>
+        <v>109</v>
       </c>
       <c r="B45" t="s" s="270">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C45" t="s" s="271">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D45" t="s" s="272">
-        <v>190</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s" s="273">
-        <v>191</v>
+        <v>110</v>
       </c>
       <c r="F45" t="s" s="274">
-        <v>192</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="275">
-        <v>193</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s" s="276">
-        <v>277</v>
+        <v>191</v>
       </c>
       <c r="C46" t="s" s="277">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D46" t="s" s="278">
         <v>33</v>
       </c>
       <c r="E46" t="s" s="279">
-        <v>195</v>
+        <v>113</v>
       </c>
       <c r="F46" t="s" s="280">
-        <v>196</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="281">
-        <v>197</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s" s="282">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C47" t="s" s="283">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s" s="284">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s" s="285">
         <v>117</v>
       </c>
-      <c r="D47" t="s" s="284">
-        <v>199</v>
-      </c>
-      <c r="E47" t="s" s="285">
-        <v>200</v>
-      </c>
       <c r="F47" t="s" s="286">
-        <v>201</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="287">
-        <v>202</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s" s="288">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C48" t="s" s="289">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D48" t="s" s="290">
-        <v>203</v>
+        <v>82</v>
       </c>
       <c r="E48" t="s" s="291">
-        <v>204</v>
+        <v>121</v>
       </c>
       <c r="F48" t="s" s="292">
-        <v>205</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="293">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s" s="294">
-        <v>278</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s" s="295">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D49" t="s" s="296">
         <v>33</v>
       </c>
       <c r="E49" t="s" s="297">
-        <v>208</v>
+        <v>125</v>
       </c>
       <c r="F49" t="s" s="298">
-        <v>209</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="299">
-        <v>210</v>
+        <v>127</v>
       </c>
       <c r="B50" t="s" s="300">
-        <v>279</v>
+        <v>197</v>
       </c>
       <c r="C50" t="s" s="301">
         <v>14</v>
       </c>
       <c r="D50" t="s" s="302">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="E50" t="s" s="303">
-        <v>213</v>
+        <v>129</v>
       </c>
       <c r="F50" t="s" s="304">
-        <v>214</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="305">
-        <v>215</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s" s="306">
-        <v>280</v>
+        <v>198</v>
       </c>
       <c r="C51" t="s" s="307">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D51" t="s" s="308">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E51" t="s" s="309">
-        <v>217</v>
+        <v>133</v>
       </c>
       <c r="F51" t="s" s="310">
-        <v>218</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="311">
-        <v>219</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s" s="312">
-        <v>281</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s" s="313">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D52" t="s" s="314">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E52" t="s" s="315">
-        <v>221</v>
+        <v>137</v>
       </c>
       <c r="F52" t="s" s="316">
-        <v>222</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="317">
-        <v>223</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s" s="318">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="C53" t="s" s="319">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D53" t="s" s="320">
-        <v>224</v>
+        <v>103</v>
       </c>
       <c r="E53" t="s" s="321">
-        <v>225</v>
+        <v>141</v>
       </c>
       <c r="F53" t="s" s="322">
-        <v>226</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="323">
-        <v>227</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s" s="324">
-        <v>282</v>
+        <v>200</v>
       </c>
       <c r="C54" t="s" s="325">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D54" t="s" s="326">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="E54" t="s" s="327">
-        <v>229</v>
+        <v>146</v>
       </c>
       <c r="F54" t="s" s="328">
-        <v>230</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="329">
-        <v>231</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s" s="330">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="C55" t="s" s="331">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D55" t="s" s="332">
-        <v>233</v>
+        <v>82</v>
       </c>
       <c r="E55" t="s" s="333">
-        <v>234</v>
+        <v>150</v>
       </c>
       <c r="F55" t="s" s="334">
-        <v>235</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="335">
-        <v>236</v>
+        <v>152</v>
       </c>
       <c r="B56" t="s" s="336">
-        <v>283</v>
+        <v>202</v>
       </c>
       <c r="C56" t="s" s="337">
         <v>14</v>
       </c>
       <c r="D56" t="s" s="338">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E56" t="s" s="339">
-        <v>238</v>
+        <v>154</v>
       </c>
       <c r="F56" t="s" s="340">
-        <v>239</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="341">
-        <v>240</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s" s="342">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="C57" t="s" s="343">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s" s="344">
-        <v>242</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s" s="345">
-        <v>243</v>
+        <v>158</v>
       </c>
       <c r="F57" t="s" s="346">
-        <v>244</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="347">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="B58" t="s" s="348">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="C58" t="s" s="349">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="D58" t="s" s="350">
-        <v>246</v>
+        <v>42</v>
       </c>
       <c r="E58" t="s" s="351">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="F58" t="s" s="352">
-        <v>248</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="353">
-        <v>249</v>
+        <v>164</v>
       </c>
       <c r="B59" t="s" s="354">
-        <v>284</v>
+        <v>205</v>
       </c>
       <c r="C59" t="s" s="355">
         <v>14</v>
       </c>
       <c r="D59" t="s" s="356">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="E59" t="s" s="357">
-        <v>251</v>
+        <v>166</v>
       </c>
       <c r="F59" t="s" s="358">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="359">
-        <v>253</v>
+        <v>168</v>
       </c>
       <c r="B60" t="s" s="360">
-        <v>285</v>
+        <v>206</v>
       </c>
       <c r="C60" t="s" s="361">
         <v>14</v>
       </c>
       <c r="D60" t="s" s="362">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E60" t="s" s="363">
-        <v>255</v>
+        <v>170</v>
       </c>
       <c r="F60" t="s" s="364">
-        <v>256</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="365">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="B61" t="s" s="366">
-        <v>286</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s" s="367">
         <v>14</v>
       </c>
       <c r="D61" t="s" s="368">
+        <v>42</v>
+      </c>
+      <c r="E61" t="s" s="369">
+        <v>174</v>
+      </c>
+      <c r="F61" t="s" s="370">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="371">
+        <v>97</v>
+      </c>
+      <c r="B62" t="s" s="372">
+        <v>192</v>
+      </c>
+      <c r="C62" t="s" s="373">
+        <v>14</v>
+      </c>
+      <c r="D62" t="s" s="374">
+        <v>20</v>
+      </c>
+      <c r="E62" t="s" s="375">
+        <v>99</v>
+      </c>
+      <c r="F62" t="s" s="376">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="377">
         <v>101</v>
       </c>
-      <c r="E61" t="s" s="369">
-        <v>259</v>
-      </c>
-      <c r="F61" t="s" s="370">
-        <v>260</v>
+      <c r="B63" t="s" s="378">
+        <v>193</v>
+      </c>
+      <c r="C63" t="s" s="379">
+        <v>14</v>
+      </c>
+      <c r="D63" t="s" s="380">
+        <v>103</v>
+      </c>
+      <c r="E63" t="s" s="381">
+        <v>104</v>
+      </c>
+      <c r="F63" t="s" s="382">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="383">
+        <v>106</v>
+      </c>
+      <c r="B64" t="s" s="384">
+        <v>193</v>
+      </c>
+      <c r="C64" t="s" s="385">
+        <v>14</v>
+      </c>
+      <c r="D64" t="s" s="386">
+        <v>82</v>
+      </c>
+      <c r="E64" t="s" s="387">
+        <v>107</v>
+      </c>
+      <c r="F64" t="s" s="388">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="389">
+        <v>109</v>
+      </c>
+      <c r="B65" t="s" s="390">
+        <v>192</v>
+      </c>
+      <c r="C65" t="s" s="391">
+        <v>14</v>
+      </c>
+      <c r="D65" t="s" s="392">
+        <v>15</v>
+      </c>
+      <c r="E65" t="s" s="393">
+        <v>110</v>
+      </c>
+      <c r="F65" t="s" s="394">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="395">
+        <v>112</v>
+      </c>
+      <c r="B66" t="s" s="396">
+        <v>191</v>
+      </c>
+      <c r="C66" t="s" s="397">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s" s="398">
+        <v>33</v>
+      </c>
+      <c r="E66" t="s" s="399">
+        <v>113</v>
+      </c>
+      <c r="F66" t="s" s="400">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="401">
+        <v>115</v>
+      </c>
+      <c r="B67" t="s" s="402">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s" s="403">
+        <v>14</v>
+      </c>
+      <c r="D67" t="s" s="404">
+        <v>20</v>
+      </c>
+      <c r="E67" t="s" s="405">
+        <v>117</v>
+      </c>
+      <c r="F67" t="s" s="406">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="407">
+        <v>119</v>
+      </c>
+      <c r="B68" t="s" s="408">
+        <v>195</v>
+      </c>
+      <c r="C68" t="s" s="409">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s" s="410">
+        <v>82</v>
+      </c>
+      <c r="E68" t="s" s="411">
+        <v>121</v>
+      </c>
+      <c r="F68" t="s" s="412">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="413">
+        <v>123</v>
+      </c>
+      <c r="B69" t="s" s="414">
+        <v>196</v>
+      </c>
+      <c r="C69" t="s" s="415">
+        <v>14</v>
+      </c>
+      <c r="D69" t="s" s="416">
+        <v>33</v>
+      </c>
+      <c r="E69" t="s" s="417">
+        <v>125</v>
+      </c>
+      <c r="F69" t="s" s="418">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="419">
+        <v>127</v>
+      </c>
+      <c r="B70" t="s" s="420">
+        <v>197</v>
+      </c>
+      <c r="C70" t="s" s="421">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s" s="422">
+        <v>15</v>
+      </c>
+      <c r="E70" t="s" s="423">
+        <v>129</v>
+      </c>
+      <c r="F70" t="s" s="424">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="425">
+        <v>131</v>
+      </c>
+      <c r="B71" t="s" s="426">
+        <v>198</v>
+      </c>
+      <c r="C71" t="s" s="427">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s" s="428">
+        <v>42</v>
+      </c>
+      <c r="E71" t="s" s="429">
+        <v>133</v>
+      </c>
+      <c r="F71" t="s" s="430">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="431">
+        <v>135</v>
+      </c>
+      <c r="B72" t="s" s="432">
+        <v>50</v>
+      </c>
+      <c r="C72" t="s" s="433">
+        <v>51</v>
+      </c>
+      <c r="D72" t="s" s="434">
+        <v>136</v>
+      </c>
+      <c r="E72" t="s" s="435">
+        <v>137</v>
+      </c>
+      <c r="F72" t="s" s="436">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="437">
+        <v>139</v>
+      </c>
+      <c r="B73" t="s" s="438">
+        <v>199</v>
+      </c>
+      <c r="C73" t="s" s="439">
+        <v>14</v>
+      </c>
+      <c r="D73" t="s" s="440">
+        <v>103</v>
+      </c>
+      <c r="E73" t="s" s="441">
+        <v>141</v>
+      </c>
+      <c r="F73" t="s" s="442">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="443">
+        <v>143</v>
+      </c>
+      <c r="B74" t="s" s="444">
+        <v>200</v>
+      </c>
+      <c r="C74" t="s" s="445">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s" s="446">
+        <v>145</v>
+      </c>
+      <c r="E74" t="s" s="447">
+        <v>146</v>
+      </c>
+      <c r="F74" t="s" s="448">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="449">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s" s="450">
+        <v>201</v>
+      </c>
+      <c r="C75" t="s" s="451">
+        <v>14</v>
+      </c>
+      <c r="D75" t="s" s="452">
+        <v>82</v>
+      </c>
+      <c r="E75" t="s" s="453">
+        <v>150</v>
+      </c>
+      <c r="F75" t="s" s="454">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="455">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s" s="456">
+        <v>202</v>
+      </c>
+      <c r="C76" t="s" s="457">
+        <v>14</v>
+      </c>
+      <c r="D76" t="s" s="458">
+        <v>33</v>
+      </c>
+      <c r="E76" t="s" s="459">
+        <v>154</v>
+      </c>
+      <c r="F76" t="s" s="460">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="461">
+        <v>156</v>
+      </c>
+      <c r="B77" t="s" s="462">
+        <v>203</v>
+      </c>
+      <c r="C77" t="s" s="463">
+        <v>14</v>
+      </c>
+      <c r="D77" t="s" s="464">
+        <v>20</v>
+      </c>
+      <c r="E77" t="s" s="465">
+        <v>158</v>
+      </c>
+      <c r="F77" t="s" s="466">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="467">
+        <v>160</v>
+      </c>
+      <c r="B78" t="s" s="468">
+        <v>204</v>
+      </c>
+      <c r="C78" t="s" s="469">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s" s="470">
+        <v>42</v>
+      </c>
+      <c r="E78" t="s" s="471">
+        <v>162</v>
+      </c>
+      <c r="F78" t="s" s="472">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="473">
+        <v>164</v>
+      </c>
+      <c r="B79" t="s" s="474">
+        <v>205</v>
+      </c>
+      <c r="C79" t="s" s="475">
+        <v>14</v>
+      </c>
+      <c r="D79" t="s" s="476">
+        <v>33</v>
+      </c>
+      <c r="E79" t="s" s="477">
+        <v>166</v>
+      </c>
+      <c r="F79" t="s" s="478">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="479">
+        <v>168</v>
+      </c>
+      <c r="B80" t="s" s="480">
+        <v>206</v>
+      </c>
+      <c r="C80" t="s" s="481">
+        <v>14</v>
+      </c>
+      <c r="D80" t="s" s="482">
+        <v>61</v>
+      </c>
+      <c r="E80" t="s" s="483">
+        <v>170</v>
+      </c>
+      <c r="F80" t="s" s="484">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="485">
+        <v>172</v>
+      </c>
+      <c r="B81" t="s" s="486">
+        <v>207</v>
+      </c>
+      <c r="C81" t="s" s="487">
+        <v>14</v>
+      </c>
+      <c r="D81" t="s" s="488">
+        <v>42</v>
+      </c>
+      <c r="E81" t="s" s="489">
+        <v>174</v>
+      </c>
+      <c r="F81" t="s" s="490">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>